<commit_message>
Fix detection Value formula
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/17_Workflow.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/17_Workflow.xlsx
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="42">
   <si>
     <t>Action</t>
   </si>
@@ -332,6 +332,21 @@
   </si>
   <si>
     <t>Workspace_Plan</t>
+  </si>
+  <si>
+    <t>Update Customer Table Source</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Update Customer Table Output</t>
+  </si>
+  <si>
+    <t>return LIB_EWS.UpdateCustomerUnitSource();</t>
+  </si>
+  <si>
+    <t>LIB_EWS.UpdateCustomerUnitOutput();</t>
   </si>
 </sst>
 </file>
@@ -472,13 +487,15 @@
       <name val="Trebuchet MS"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Trebuchet MS"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,18 +505,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFAC2524"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -515,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -578,10 +583,6 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,6 +837,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9572625"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1076,6 +1125,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 7"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8629650" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1316,6 +1413,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10153650" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1524,6 +1669,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="5" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1858,10 +2051,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A2" sqref="A2:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1918,87 +2111,151 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>17</v>
+      <c r="D2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="24" t="s">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" t="s">
         <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" t="s">
         <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" t="s">
         <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>31</v>
+      <c r="B6" t="s">
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D8" t="s">
         <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2010,10 +2267,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2021,7 +2278,7 @@
     <col min="1" max="1" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2046,27 +2303,27 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>20</v>
+      <c r="B2" t="s">
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>20</v>
+      <c r="B3" t="s">
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2074,7 +2331,7 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
@@ -2088,13 +2345,13 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>15</v>
+      <c r="B5" t="s">
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2102,63 +2359,63 @@
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>19</v>
+      <c r="B6" t="s">
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>19</v>
+      <c r="B7" t="s">
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="24" t="s">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>29</v>
+      <c r="D9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" t="s">
         <v>30</v>
       </c>
       <c r="C10" t="s">
@@ -2169,31 +2426,59 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>30</v>
+      <c r="B11" t="s">
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>31</v>
+      <c r="B12" t="s">
+        <v>19</v>
       </c>
       <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
+      <c r="D14" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD CCR Default BIB
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/17_Workflow.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/17_Workflow.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Global Variables" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Parameters!$A$1:$E$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Parameters!$A$1:$E$14</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -328,9 +328,6 @@
     <t>[Commons] Evaluate Formula</t>
   </si>
   <si>
-    <t>LIB_EWS.UpdateWorkpalceTableAll();</t>
-  </si>
-  <si>
     <t>Workspace_Plan</t>
   </si>
   <si>
@@ -346,14 +343,17 @@
     <t>return LIB_EWS.UpdateCustomerUnitSource();</t>
   </si>
   <si>
-    <t>LIB_EWS.UpdateCustomerUnitOutput();</t>
+    <t>return LIB_EWS.UpdateCustomerUnitOutput();</t>
+  </si>
+  <si>
+    <t>return LIB_EWS.UpdateWorkpalceTableAll();</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -485,14 +485,6 @@
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Trebuchet MS"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -885,6 +877,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9572625"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1173,6 +1213,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 7"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8629650" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1461,6 +1549,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10782300" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1717,6 +1853,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2115,7 +2299,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -2138,10 +2322,10 @@
         <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -2158,7 +2342,7 @@
         <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -2178,7 +2362,7 @@
         <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" t="s">
         <v>15</v>
@@ -2212,7 +2396,7 @@
         <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J7" t="s">
         <v>15</v>
@@ -2232,7 +2416,7 @@
         <v>17</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" t="s">
         <v>15</v>
@@ -2243,7 +2427,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -2252,7 +2436,7 @@
         <v>34</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
@@ -2267,10 +2451,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2304,16 +2489,16 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2327,7 +2512,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2341,7 +2526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2355,7 +2540,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2369,7 +2554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2383,7 +2568,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2397,7 +2582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2408,10 +2593,10 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2436,10 +2621,10 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2453,7 +2638,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2472,17 +2657,22 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E9">
+  <autoFilter ref="A1:E14">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="formula"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:E16">
       <sortCondition ref="B1:B16"/>
     </sortState>

</xml_diff>

<commit_message>
Add formula to update predictive modules
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/17_Workflow.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/17_Workflow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Global Variables" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Parameters!$A$1:$E$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Parameters!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="43">
   <si>
     <t>Action</t>
   </si>
@@ -344,12 +344,18 @@
   </si>
   <si>
     <t>return LIB_EWS.UpdateWorkpalceTableAll();</t>
+  </si>
+  <si>
+    <t>Update predictive Model</t>
+  </si>
+  <si>
+    <t>return LIB_EWS.UpdatePredictiveModel();</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -970,70 +976,22 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2055" name="_xssf_cell_comment" hidden="1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 7"/>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1041,7 +999,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:ext cx="9525000" cy="9572625"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1066,6 +1024,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2055" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1081,7 +1087,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 7"/>
+        <xdr:cNvPr id="2" name="AutoShape 7"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1129,7 +1135,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 7"/>
+        <xdr:cNvPr id="3" name="AutoShape 7"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1137,7 +1143,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11420475" cy="9525000"/>
+          <a:ext cx="9525000" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1177,7 +1183,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 7"/>
+        <xdr:cNvPr id="4" name="AutoShape 7"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1185,7 +1191,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8515350" cy="9525000"/>
+          <a:ext cx="11420475" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1220,12 +1226,12 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 7"/>
+        <xdr:cNvPr id="5" name="AutoShape 7"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1233,7 +1239,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8629650" cy="9525000"/>
+          <a:ext cx="8515350" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1273,7 +1279,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 7"/>
+        <xdr:cNvPr id="6" name="AutoShape 7"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1321,7 +1327,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 7"/>
+        <xdr:cNvPr id="7" name="AutoShape 7"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1354,11 +1360,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1369,55 +1370,12 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3075" name="_xssf_cell_comment" hidden="1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 3"/>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 7"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1425,7 +1383,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:ext cx="8629650" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1460,12 +1418,12 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 3"/>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 7"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1473,7 +1431,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:ext cx="8629650" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1498,6 +1456,11 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1508,12 +1471,55 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 3"/>
+        <xdr:cNvPr id="3075" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1521,7 +1527,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9448800" cy="9525000"/>
+          <a:ext cx="9525000" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1556,12 +1562,12 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 3"/>
+        <xdr:cNvPr id="3" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1569,7 +1575,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9448800" cy="9525000"/>
+          <a:ext cx="9525000" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1604,12 +1610,12 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 3"/>
+        <xdr:cNvPr id="4" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1617,7 +1623,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10153650" cy="9525000"/>
+          <a:ext cx="9448800" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1652,12 +1658,12 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 3"/>
+        <xdr:cNvPr id="5" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1665,7 +1671,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10782300" cy="9525000"/>
+          <a:ext cx="9448800" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1700,12 +1706,12 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 3"/>
+        <xdr:cNvPr id="6" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1713,7 +1719,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10782300" cy="7524750"/>
+          <a:ext cx="10153650" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1738,70 +1744,22 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>47</xdr:row>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4099" name="_xssf_cell_comment" hidden="1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 3"/>
+        <xdr:cNvPr id="7" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1809,7 +1767,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:ext cx="10782300" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1842,14 +1800,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 3"/>
+        <xdr:cNvPr id="8" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1857,7 +1815,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:ext cx="10782300" cy="7524750"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1890,14 +1848,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 3"/>
+        <xdr:cNvPr id="9" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1905,7 +1863,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:ext cx="10782300" cy="7524750"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1930,6 +1888,11 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1945,7 +1908,50 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 3"/>
+        <xdr:cNvPr id="4099" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1993,7 +1999,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 3"/>
+        <xdr:cNvPr id="3" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2041,7 +2047,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 3"/>
+        <xdr:cNvPr id="4" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2089,7 +2095,199 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2201,6 +2399,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2236,6 +2451,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2426,7 +2658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3:J9"/>
     </sheetView>
   </sheetViews>
@@ -2605,11 +2837,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2652,7 +2883,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2666,7 +2897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2680,7 +2911,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2694,7 +2925,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2708,7 +2939,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2722,7 +2953,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2736,21 +2967,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2758,10 +2989,10 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -2769,30 +3000,30 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2800,10 +3031,10 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2811,22 +3042,31 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>37</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E14">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="formula"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:E15">
     <sortState ref="A2:E16">
       <sortCondition ref="B1:B16"/>
     </sortState>

</xml_diff>